<commit_message>
zaj5 and fizyka update
w koncu xd
</commit_message>
<xml_diff>
--- a/fizyka_lab/obliczenia.xlsx
+++ b/fizyka_lab/obliczenia.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="89">
   <si>
     <t>Lp.</t>
   </si>
@@ -639,20 +639,208 @@
   <si>
     <t>Ex[V]/I[A]</t>
   </si>
+  <si>
+    <t>s[m]</t>
+  </si>
+  <si>
+    <t>t[s]</t>
+  </si>
+  <si>
+    <t>r[m]</t>
+  </si>
+  <si>
+    <t>R[m]</t>
+  </si>
+  <si>
+    <t>D[m]</t>
+  </si>
+  <si>
+    <t>ρk [kg/m3]</t>
+  </si>
+  <si>
+    <r>
+      <t>ρ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>c</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [kg/m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>η</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">i </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[Pa·s]</t>
+    </r>
+  </si>
+  <si>
+    <t>L.p.</t>
+  </si>
+  <si>
+    <t>D[cm]</t>
+  </si>
+  <si>
+    <t>d[mm]</t>
+  </si>
+  <si>
+    <t>r[mm]</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Masa N kulek [g]</t>
+  </si>
+  <si>
+    <t>pk</t>
+  </si>
+  <si>
+    <t>srednia:</t>
+  </si>
+  <si>
+    <t>g[m/s^2]</t>
+  </si>
+  <si>
+    <t>pi</t>
+  </si>
+  <si>
+    <t>r/R</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>pk-pc</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>r^2</t>
+  </si>
+  <si>
+    <t>Masa N kulek[kg]</t>
+  </si>
+  <si>
+    <t>średnie r</t>
+  </si>
+  <si>
+    <t>ηi [Pa·s]</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>η[%]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>Δ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>η</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000000000000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -733,7 +921,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -1027,11 +1215,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1041,22 +1240,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1067,9 +1266,23 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1085,10 +1298,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1103,13 +1316,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -2528,15 +2749,15 @@
       <c r="G4" t="s">
         <v>18</v>
       </c>
-      <c r="N4" s="32" t="s">
+      <c r="N4" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="O4" s="32"/>
-      <c r="P4" s="32"/>
-      <c r="Q4" s="32"/>
-      <c r="R4" s="32"/>
-      <c r="S4" s="32"/>
-      <c r="T4" s="32"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="40"/>
+      <c r="Q4" s="40"/>
+      <c r="R4" s="40"/>
+      <c r="S4" s="40"/>
+      <c r="T4" s="40"/>
     </row>
     <row r="6" spans="4:20" ht="18.75" x14ac:dyDescent="0.35">
       <c r="D6" t="s">
@@ -2903,33 +3124,33 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="4" spans="4:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="O4" s="33" t="s">
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="O4" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="P4" s="33"/>
-      <c r="Q4" s="33"/>
-      <c r="R4" s="33"/>
-      <c r="S4" s="33"/>
-      <c r="T4" s="33"/>
-      <c r="U4" s="33"/>
-      <c r="V4" s="33"/>
-      <c r="X4" s="33" t="s">
+      <c r="P4" s="41"/>
+      <c r="Q4" s="41"/>
+      <c r="R4" s="41"/>
+      <c r="S4" s="41"/>
+      <c r="T4" s="41"/>
+      <c r="U4" s="41"/>
+      <c r="V4" s="41"/>
+      <c r="X4" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="Y4" s="33"/>
-      <c r="Z4" s="33"/>
-      <c r="AA4" s="33"/>
-      <c r="AB4" s="33"/>
-      <c r="AC4" s="33"/>
+      <c r="Y4" s="41"/>
+      <c r="Z4" s="41"/>
+      <c r="AA4" s="41"/>
+      <c r="AB4" s="41"/>
+      <c r="AC4" s="41"/>
     </row>
     <row r="5" spans="4:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
@@ -3953,7 +4174,7 @@
       <c r="A4" s="20"/>
       <c r="B4" s="20"/>
       <c r="C4" s="20"/>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="42" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="28" t="s">
@@ -3968,7 +4189,7 @@
       <c r="H4" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="34" t="s">
+      <c r="I4" s="42" t="s">
         <v>31</v>
       </c>
       <c r="J4" s="20"/>
@@ -4008,16 +4229,16 @@
       <c r="X4" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="Y4" s="38" t="s">
+      <c r="Y4" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="Z4" s="38"/>
+      <c r="Z4" s="46"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
       <c r="B5" s="20"/>
       <c r="C5" s="20"/>
-      <c r="D5" s="35"/>
+      <c r="D5" s="43"/>
       <c r="E5" s="3">
         <v>1</v>
       </c>
@@ -4031,7 +4252,7 @@
         <f>G5*(F5/(E5-F5))</f>
         <v>129.85714285714286</v>
       </c>
-      <c r="I5" s="35"/>
+      <c r="I5" s="43"/>
       <c r="J5" s="20"/>
       <c r="K5" s="5">
         <v>1</v>
@@ -4073,16 +4294,16 @@
       </c>
       <c r="W5" s="20"/>
       <c r="X5" s="20"/>
-      <c r="Y5" s="37" t="s">
+      <c r="Y5" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="Z5" s="37"/>
+      <c r="Z5" s="45"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="20"/>
       <c r="B6" s="20"/>
       <c r="C6" s="20"/>
-      <c r="D6" s="35"/>
+      <c r="D6" s="43"/>
       <c r="E6" s="3">
         <v>1</v>
       </c>
@@ -4096,7 +4317,7 @@
         <f t="shared" ref="H6:H13" si="0">G6*(F6/(E6-F6))</f>
         <v>148.61538461538461</v>
       </c>
-      <c r="I6" s="35"/>
+      <c r="I6" s="43"/>
       <c r="J6" s="20"/>
       <c r="K6" s="5">
         <v>2</v>
@@ -4136,7 +4357,7 @@
       <c r="A7" s="20"/>
       <c r="B7" s="20"/>
       <c r="C7" s="20"/>
-      <c r="D7" s="36"/>
+      <c r="D7" s="44"/>
       <c r="E7" s="3">
         <v>1</v>
       </c>
@@ -4569,7 +4790,7 @@
       <c r="Z15" s="20"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D16" s="34" t="s">
+      <c r="D16" s="42" t="s">
         <v>37</v>
       </c>
       <c r="E16" s="28" t="s">
@@ -4584,7 +4805,7 @@
       <c r="H16" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="I16" s="34" t="s">
+      <c r="I16" s="42" t="s">
         <v>31</v>
       </c>
       <c r="K16" s="5" t="s">
@@ -4607,7 +4828,7 @@
       </c>
     </row>
     <row r="17" spans="4:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="35"/>
+      <c r="D17" s="43"/>
       <c r="E17" s="3"/>
       <c r="F17" s="4">
         <v>0.3</v>
@@ -4617,7 +4838,7 @@
         <f>G17*(F17/(E17-F17))</f>
         <v>0</v>
       </c>
-      <c r="I17" s="35"/>
+      <c r="I17" s="43"/>
       <c r="K17" s="5">
         <v>1</v>
       </c>
@@ -4643,7 +4864,7 @@
       </c>
     </row>
     <row r="18" spans="4:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D18" s="35"/>
+      <c r="D18" s="43"/>
       <c r="E18" s="2"/>
       <c r="F18" s="1">
         <v>0.35</v>
@@ -4653,7 +4874,7 @@
         <f t="shared" ref="H18:H25" si="6">G18*(F18/(E18-F18))</f>
         <v>0</v>
       </c>
-      <c r="I18" s="35"/>
+      <c r="I18" s="43"/>
       <c r="K18" s="5">
         <v>2</v>
       </c>
@@ -4679,7 +4900,7 @@
       </c>
     </row>
     <row r="19" spans="4:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D19" s="36"/>
+      <c r="D19" s="44"/>
       <c r="E19" s="2"/>
       <c r="F19" s="1">
         <v>0.4</v>
@@ -4948,7 +5169,7 @@
     </row>
     <row r="27" spans="4:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="4:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D28" s="34" t="s">
+      <c r="D28" s="42" t="s">
         <v>38</v>
       </c>
       <c r="E28" s="28" t="s">
@@ -4963,7 +5184,7 @@
       <c r="H28" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="I28" s="34" t="s">
+      <c r="I28" s="42" t="s">
         <v>31</v>
       </c>
       <c r="K28" s="5" t="s">
@@ -4986,7 +5207,7 @@
       </c>
     </row>
     <row r="29" spans="4:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D29" s="35"/>
+      <c r="D29" s="43"/>
       <c r="E29" s="3"/>
       <c r="F29" s="4">
         <v>0.3</v>
@@ -4996,7 +5217,7 @@
         <f>G29*(F29/(E29-F29))</f>
         <v>0</v>
       </c>
-      <c r="I29" s="35"/>
+      <c r="I29" s="43"/>
       <c r="K29" s="5">
         <v>1</v>
       </c>
@@ -5022,7 +5243,7 @@
       </c>
     </row>
     <row r="30" spans="4:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D30" s="35"/>
+      <c r="D30" s="43"/>
       <c r="E30" s="2"/>
       <c r="F30" s="1">
         <v>0.35</v>
@@ -5032,7 +5253,7 @@
         <f t="shared" ref="H30:H37" si="13">G30*(F30/(E30-F30))</f>
         <v>0</v>
       </c>
-      <c r="I30" s="35"/>
+      <c r="I30" s="43"/>
       <c r="K30" s="5">
         <v>2</v>
       </c>
@@ -5058,7 +5279,7 @@
       </c>
     </row>
     <row r="31" spans="4:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D31" s="36"/>
+      <c r="D31" s="44"/>
       <c r="E31" s="2"/>
       <c r="F31" s="1">
         <v>0.4</v>
@@ -5327,7 +5548,7 @@
     </row>
     <row r="39" spans="4:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="40" spans="4:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D40" s="34" t="s">
+      <c r="D40" s="42" t="s">
         <v>39</v>
       </c>
       <c r="E40" s="28" t="s">
@@ -5342,7 +5563,7 @@
       <c r="H40" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="I40" s="34" t="s">
+      <c r="I40" s="42" t="s">
         <v>31</v>
       </c>
       <c r="K40" s="5" t="s">
@@ -5365,7 +5586,7 @@
       </c>
     </row>
     <row r="41" spans="4:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D41" s="35"/>
+      <c r="D41" s="43"/>
       <c r="E41" s="3"/>
       <c r="F41" s="4">
         <v>0.3</v>
@@ -5375,7 +5596,7 @@
         <f>G41*(F41/(E41-F41))</f>
         <v>0</v>
       </c>
-      <c r="I41" s="35"/>
+      <c r="I41" s="43"/>
       <c r="K41" s="5">
         <v>1</v>
       </c>
@@ -5401,7 +5622,7 @@
       </c>
     </row>
     <row r="42" spans="4:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D42" s="35"/>
+      <c r="D42" s="43"/>
       <c r="E42" s="2"/>
       <c r="F42" s="1">
         <v>0.35</v>
@@ -5411,7 +5632,7 @@
         <f t="shared" ref="H42:H49" si="20">G42*(F42/(E42-F42))</f>
         <v>0</v>
       </c>
-      <c r="I42" s="35"/>
+      <c r="I42" s="43"/>
       <c r="K42" s="5">
         <v>2</v>
       </c>
@@ -5437,7 +5658,7 @@
       </c>
     </row>
     <row r="43" spans="4:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D43" s="36"/>
+      <c r="D43" s="44"/>
       <c r="E43" s="2"/>
       <c r="F43" s="1">
         <v>0.4</v>
@@ -5738,7 +5959,7 @@
   <sheetData>
     <row r="3" spans="4:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="4:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="49" t="s">
         <v>48</v>
       </c>
       <c r="E4" s="30" t="s">
@@ -5771,12 +5992,12 @@
       <c r="Q4" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="S4" s="45" t="s">
+      <c r="S4" s="34" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="5" spans="4:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="42"/>
+      <c r="D5" s="50"/>
       <c r="E5" s="3">
         <v>5.0600000000000005E-4</v>
       </c>
@@ -5787,25 +6008,25 @@
         <f>ROUND(E5*F5,4)</f>
         <v>4.6299000000000001</v>
       </c>
-      <c r="H5" s="39">
+      <c r="H5" s="47">
         <f>ROUND(AVERAGE(G5:G14),4)</f>
         <v>4.4474999999999998</v>
       </c>
-      <c r="J5" s="43"/>
-      <c r="K5" s="43"/>
-      <c r="L5" s="44">
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="33">
         <f>G5</f>
         <v>4.6299000000000001</v>
       </c>
-      <c r="M5" s="44">
+      <c r="M5" s="33">
         <f>F5</f>
         <v>9150</v>
       </c>
-      <c r="N5" s="44">
+      <c r="N5" s="33">
         <f>E5</f>
         <v>5.0600000000000005E-4</v>
       </c>
-      <c r="O5" s="44">
+      <c r="O5" s="33">
         <f>(0.8/100*E5)+0.00001</f>
         <v>1.4048000000000002E-5</v>
       </c>
@@ -5822,7 +6043,7 @@
       </c>
     </row>
     <row r="6" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D6" s="39">
+      <c r="D6" s="47">
         <v>1</v>
       </c>
       <c r="E6" s="1">
@@ -5835,22 +6056,22 @@
         <f t="shared" ref="G6:G14" si="0">ROUND(E6*F6,4)</f>
         <v>4.6327999999999996</v>
       </c>
-      <c r="H6" s="40"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
-      <c r="L6" s="44">
+      <c r="H6" s="48"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="33">
         <f t="shared" ref="L6:L14" si="1">G6</f>
         <v>4.6327999999999996</v>
       </c>
-      <c r="M6" s="44">
+      <c r="M6" s="33">
         <f t="shared" ref="M6:M14" si="2">F6</f>
         <v>6590</v>
       </c>
-      <c r="N6" s="44">
+      <c r="N6" s="33">
         <f t="shared" ref="N6:N14" si="3">E6</f>
         <v>7.0299999999999996E-4</v>
       </c>
-      <c r="O6" s="44">
+      <c r="O6" s="33">
         <f t="shared" ref="O6:O14" si="4">(0.8/100*E6)+0.00001</f>
         <v>1.5624000000000002E-5</v>
       </c>
@@ -5864,7 +6085,7 @@
       </c>
     </row>
     <row r="7" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D7" s="40"/>
+      <c r="D7" s="48"/>
       <c r="E7" s="1">
         <v>8.3699999999999996E-4</v>
       </c>
@@ -5875,22 +6096,22 @@
         <f t="shared" si="0"/>
         <v>4.6243999999999996</v>
       </c>
-      <c r="H7" s="40"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="43"/>
-      <c r="L7" s="44">
+      <c r="H7" s="48"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="33">
         <f t="shared" si="1"/>
         <v>4.6243999999999996</v>
       </c>
-      <c r="M7" s="44">
+      <c r="M7" s="33">
         <f t="shared" si="2"/>
         <v>5525</v>
       </c>
-      <c r="N7" s="44">
+      <c r="N7" s="33">
         <f t="shared" si="3"/>
         <v>8.3699999999999996E-4</v>
       </c>
-      <c r="O7" s="44">
+      <c r="O7" s="33">
         <f t="shared" si="4"/>
         <v>1.6696000000000001E-5</v>
       </c>
@@ -5904,7 +6125,7 @@
       </c>
     </row>
     <row r="8" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D8" s="40"/>
+      <c r="D8" s="48"/>
       <c r="E8" s="1">
         <v>1.0790000000000001E-3</v>
       </c>
@@ -5915,22 +6136,22 @@
         <f t="shared" si="0"/>
         <v>4.6342999999999996</v>
       </c>
-      <c r="H8" s="40"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="43"/>
-      <c r="L8" s="44">
+      <c r="H8" s="48"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="33">
         <f t="shared" si="1"/>
         <v>4.6342999999999996</v>
       </c>
-      <c r="M8" s="44">
+      <c r="M8" s="33">
         <f t="shared" si="2"/>
         <v>4295</v>
       </c>
-      <c r="N8" s="44">
+      <c r="N8" s="33">
         <f t="shared" si="3"/>
         <v>1.0790000000000001E-3</v>
       </c>
-      <c r="O8" s="44">
+      <c r="O8" s="33">
         <f t="shared" si="4"/>
         <v>1.8632000000000001E-5</v>
       </c>
@@ -5944,7 +6165,7 @@
       </c>
     </row>
     <row r="9" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D9" s="40"/>
+      <c r="D9" s="48"/>
       <c r="E9" s="1">
         <v>1.1640000000000001E-3</v>
       </c>
@@ -5955,22 +6176,22 @@
         <f t="shared" si="0"/>
         <v>4.6326999999999998</v>
       </c>
-      <c r="H9" s="40"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="43"/>
-      <c r="L9" s="44">
+      <c r="H9" s="48"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="33">
         <f t="shared" si="1"/>
         <v>4.6326999999999998</v>
       </c>
-      <c r="M9" s="44">
+      <c r="M9" s="33">
         <f t="shared" si="2"/>
         <v>3980</v>
       </c>
-      <c r="N9" s="44">
+      <c r="N9" s="33">
         <f t="shared" si="3"/>
         <v>1.1640000000000001E-3</v>
       </c>
-      <c r="O9" s="44">
+      <c r="O9" s="33">
         <f t="shared" si="4"/>
         <v>1.9312000000000001E-5</v>
       </c>
@@ -5984,7 +6205,7 @@
       </c>
     </row>
     <row r="10" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D10" s="40"/>
+      <c r="D10" s="48"/>
       <c r="E10" s="1">
         <v>1.2340000000000001E-3</v>
       </c>
@@ -5995,22 +6216,22 @@
         <f t="shared" si="0"/>
         <v>4.6275000000000004</v>
       </c>
-      <c r="H10" s="40"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="43"/>
-      <c r="L10" s="44">
+      <c r="H10" s="48"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="33">
         <f t="shared" si="1"/>
         <v>4.6275000000000004</v>
       </c>
-      <c r="M10" s="44">
+      <c r="M10" s="33">
         <f t="shared" si="2"/>
         <v>3750</v>
       </c>
-      <c r="N10" s="44">
+      <c r="N10" s="33">
         <f t="shared" si="3"/>
         <v>1.2340000000000001E-3</v>
       </c>
-      <c r="O10" s="44">
+      <c r="O10" s="33">
         <f t="shared" si="4"/>
         <v>1.9872000000000002E-5</v>
       </c>
@@ -6024,7 +6245,7 @@
       </c>
     </row>
     <row r="11" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D11" s="40"/>
+      <c r="D11" s="48"/>
       <c r="E11" s="1">
         <v>1.3465E-3</v>
       </c>
@@ -6035,22 +6256,22 @@
         <f t="shared" si="0"/>
         <v>4.6252000000000004</v>
       </c>
-      <c r="H11" s="40"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="43"/>
-      <c r="L11" s="44">
+      <c r="H11" s="48"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="33">
         <f t="shared" si="1"/>
         <v>4.6252000000000004</v>
       </c>
-      <c r="M11" s="44">
+      <c r="M11" s="33">
         <f t="shared" si="2"/>
         <v>3435</v>
       </c>
-      <c r="N11" s="44">
+      <c r="N11" s="33">
         <f t="shared" si="3"/>
         <v>1.3465E-3</v>
       </c>
-      <c r="O11" s="44">
+      <c r="O11" s="33">
         <f t="shared" si="4"/>
         <v>2.0772000000000004E-5</v>
       </c>
@@ -6064,7 +6285,7 @@
       </c>
     </row>
     <row r="12" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D12" s="40"/>
+      <c r="D12" s="48"/>
       <c r="E12" s="1">
         <v>1.5045E-3</v>
       </c>
@@ -6075,22 +6296,22 @@
         <f t="shared" si="0"/>
         <v>4.6262999999999996</v>
       </c>
-      <c r="H12" s="40"/>
-      <c r="J12" s="43"/>
-      <c r="K12" s="43"/>
-      <c r="L12" s="44">
+      <c r="H12" s="48"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="33">
         <f t="shared" si="1"/>
         <v>4.6262999999999996</v>
       </c>
-      <c r="M12" s="44">
+      <c r="M12" s="33">
         <f t="shared" si="2"/>
         <v>3075</v>
       </c>
-      <c r="N12" s="44">
+      <c r="N12" s="33">
         <f t="shared" si="3"/>
         <v>1.5045E-3</v>
       </c>
-      <c r="O12" s="44">
+      <c r="O12" s="33">
         <f t="shared" si="4"/>
         <v>2.2036E-5</v>
       </c>
@@ -6104,7 +6325,7 @@
       </c>
     </row>
     <row r="13" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D13" s="40"/>
+      <c r="D13" s="48"/>
       <c r="E13" s="1">
         <v>1.616E-3</v>
       </c>
@@ -6115,22 +6336,22 @@
         <f t="shared" si="0"/>
         <v>4.6218000000000004</v>
       </c>
-      <c r="H13" s="40"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="43"/>
-      <c r="L13" s="44">
+      <c r="H13" s="48"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="33">
         <f t="shared" si="1"/>
         <v>4.6218000000000004</v>
       </c>
-      <c r="M13" s="44">
+      <c r="M13" s="33">
         <f t="shared" si="2"/>
         <v>2860</v>
       </c>
-      <c r="N13" s="44">
+      <c r="N13" s="33">
         <f t="shared" si="3"/>
         <v>1.616E-3</v>
       </c>
-      <c r="O13" s="44">
+      <c r="O13" s="33">
         <f t="shared" si="4"/>
         <v>2.2928000000000001E-5</v>
       </c>
@@ -6144,7 +6365,7 @@
       </c>
     </row>
     <row r="14" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D14" s="40"/>
+      <c r="D14" s="48"/>
       <c r="E14" s="1">
         <v>1.825E-3</v>
       </c>
@@ -6155,22 +6376,22 @@
         <f t="shared" si="0"/>
         <v>2.8195999999999999</v>
       </c>
-      <c r="H14" s="40"/>
-      <c r="J14" s="43"/>
-      <c r="K14" s="43"/>
-      <c r="L14" s="44">
+      <c r="H14" s="48"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="32"/>
+      <c r="L14" s="33">
         <f t="shared" si="1"/>
         <v>2.8195999999999999</v>
       </c>
-      <c r="M14" s="44">
+      <c r="M14" s="33">
         <f t="shared" si="2"/>
         <v>1545</v>
       </c>
-      <c r="N14" s="44">
+      <c r="N14" s="33">
         <f t="shared" si="3"/>
         <v>1.825E-3</v>
       </c>
-      <c r="O14" s="44">
+      <c r="O14" s="33">
         <f t="shared" si="4"/>
         <v>2.4600000000000002E-5</v>
       </c>
@@ -6196,14 +6417,1340 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:T56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G44" activeCellId="1" sqref="F47 G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="3:12" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="C4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K4" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="L4" s="35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="54"/>
+      <c r="E5" s="1">
+        <v>5.82</v>
+      </c>
+      <c r="F5" s="54"/>
+      <c r="G5" s="1">
+        <v>5.8</v>
+      </c>
+      <c r="H5" s="1">
+        <f>G5/2</f>
+        <v>2.9</v>
+      </c>
+      <c r="I5" s="1">
+        <v>6.34</v>
+      </c>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="D6" s="55"/>
+      <c r="E6" s="1">
+        <v>5.8</v>
+      </c>
+      <c r="F6" s="55"/>
+      <c r="G6" s="1">
+        <v>5.94</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" ref="H6:H14" si="0">G6/2</f>
+        <v>2.97</v>
+      </c>
+      <c r="I6" s="1">
+        <v>5.15</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C7" s="1">
+        <v>3</v>
+      </c>
+      <c r="D7" s="55"/>
+      <c r="E7" s="1">
+        <v>5.81</v>
+      </c>
+      <c r="F7" s="55"/>
+      <c r="G7" s="1">
+        <v>5.98</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="0"/>
+        <v>2.99</v>
+      </c>
+      <c r="I7" s="1">
+        <v>7</v>
+      </c>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C8" s="1">
+        <v>4</v>
+      </c>
+      <c r="D8" s="55"/>
+      <c r="E8" s="1">
+        <v>5.8</v>
+      </c>
+      <c r="F8" s="55"/>
+      <c r="G8" s="1">
+        <v>5.92</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="0"/>
+        <v>2.96</v>
+      </c>
+      <c r="I8" s="1">
+        <v>5.91</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C9" s="1">
+        <v>5</v>
+      </c>
+      <c r="D9" s="55"/>
+      <c r="E9" s="1">
+        <v>5.83</v>
+      </c>
+      <c r="F9" s="55"/>
+      <c r="G9" s="1">
+        <v>5.53</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="0"/>
+        <v>2.7650000000000001</v>
+      </c>
+      <c r="I9" s="1">
+        <v>6.87</v>
+      </c>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C10" s="1">
+        <v>6</v>
+      </c>
+      <c r="D10" s="55"/>
+      <c r="E10" s="1">
+        <v>5.766</v>
+      </c>
+      <c r="F10" s="55"/>
+      <c r="G10" s="1">
+        <v>5.97</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="0"/>
+        <v>2.9849999999999999</v>
+      </c>
+      <c r="I10" s="1">
+        <v>6.82</v>
+      </c>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C11" s="1">
+        <v>7</v>
+      </c>
+      <c r="D11" s="55"/>
+      <c r="E11" s="1">
+        <v>5.8120000000000003</v>
+      </c>
+      <c r="F11" s="55"/>
+      <c r="G11" s="1">
+        <v>5.87</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="0"/>
+        <v>2.9350000000000001</v>
+      </c>
+      <c r="I11" s="1">
+        <v>6.66</v>
+      </c>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C12" s="1">
+        <v>8</v>
+      </c>
+      <c r="D12" s="55"/>
+      <c r="E12" s="1">
+        <v>5.81</v>
+      </c>
+      <c r="F12" s="55"/>
+      <c r="G12" s="1">
+        <v>5.89</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" si="0"/>
+        <v>2.9449999999999998</v>
+      </c>
+      <c r="I12" s="1">
+        <v>7.56</v>
+      </c>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C13" s="1">
+        <v>9</v>
+      </c>
+      <c r="D13" s="55"/>
+      <c r="E13" s="1">
+        <v>5.7640000000000002</v>
+      </c>
+      <c r="F13" s="55"/>
+      <c r="G13" s="1">
+        <v>5.98</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="0"/>
+        <v>2.99</v>
+      </c>
+      <c r="I13" s="1">
+        <v>6.81</v>
+      </c>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C14" s="1">
+        <v>10</v>
+      </c>
+      <c r="D14" s="47"/>
+      <c r="E14" s="1">
+        <v>5.8019999999999996</v>
+      </c>
+      <c r="F14" s="47"/>
+      <c r="G14" s="1">
+        <v>5.94</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="0"/>
+        <v>2.97</v>
+      </c>
+      <c r="I14" s="1">
+        <v>5.38</v>
+      </c>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+    </row>
+    <row r="18" spans="1:20" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="C18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K18" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="L18" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="O18" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="P18" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="51">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="E19" s="1">
+        <f>E5*1/100</f>
+        <v>5.8200000000000002E-2</v>
+      </c>
+      <c r="F19" s="51">
+        <f>AVERAGE(E19:E28)</f>
+        <v>5.8013999999999996E-2</v>
+      </c>
+      <c r="G19" s="1">
+        <f>G5*1/1000</f>
+        <v>5.7999999999999996E-3</v>
+      </c>
+      <c r="H19" s="1">
+        <f>H5*1/1000</f>
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="I19" s="1">
+        <f>I5</f>
+        <v>6.34</v>
+      </c>
+      <c r="J19" s="51">
+        <f>Q19</f>
+        <v>1249.1574466594129</v>
+      </c>
+      <c r="K19" s="51">
+        <v>881.2</v>
+      </c>
+      <c r="L19" s="1">
+        <f>ROUND(I33,4)</f>
+        <v>0.1075</v>
+      </c>
+      <c r="N19" s="1">
+        <v>100</v>
+      </c>
+      <c r="O19" s="1">
+        <v>13.31</v>
+      </c>
+      <c r="P19" s="1">
+        <f>O19*1/1000</f>
+        <v>1.3310000000000001E-2</v>
+      </c>
+      <c r="Q19" s="1">
+        <f>P19/(N19*4/3*S19*POWER(H29,3))</f>
+        <v>1249.1574466594129</v>
+      </c>
+      <c r="R19" s="1">
+        <f>H29</f>
+        <v>2.941E-3</v>
+      </c>
+      <c r="S19" s="1">
+        <v>3.1415000000000002</v>
+      </c>
+      <c r="T19" s="1">
+        <v>9.8066499999999994</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C20" s="1">
+        <v>2</v>
+      </c>
+      <c r="D20" s="52"/>
+      <c r="E20" s="1">
+        <f t="shared" ref="E20:E28" si="1">E6*1/100</f>
+        <v>5.7999999999999996E-2</v>
+      </c>
+      <c r="F20" s="52"/>
+      <c r="G20" s="1">
+        <f t="shared" ref="G20:H28" si="2">G6*1/1000</f>
+        <v>5.94E-3</v>
+      </c>
+      <c r="H20" s="1">
+        <f t="shared" si="2"/>
+        <v>2.97E-3</v>
+      </c>
+      <c r="I20" s="1">
+        <f t="shared" ref="I20:I28" si="3">I6</f>
+        <v>5.15</v>
+      </c>
+      <c r="J20" s="52"/>
+      <c r="K20" s="52"/>
+      <c r="L20" s="1">
+        <f t="shared" ref="L20:L28" si="4">ROUND(I34,4)</f>
+        <v>9.1399999999999995E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C21" s="1">
+        <v>3</v>
+      </c>
+      <c r="D21" s="52"/>
+      <c r="E21" s="1">
+        <f t="shared" si="1"/>
+        <v>5.8099999999999999E-2</v>
+      </c>
+      <c r="F21" s="52"/>
+      <c r="G21" s="1">
+        <f t="shared" si="2"/>
+        <v>5.9800000000000001E-3</v>
+      </c>
+      <c r="H21" s="1">
+        <f t="shared" si="2"/>
+        <v>2.99E-3</v>
+      </c>
+      <c r="I21" s="1">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="J21" s="52"/>
+      <c r="K21" s="52"/>
+      <c r="L21" s="1">
+        <f t="shared" si="4"/>
+        <v>0.1258</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C22" s="1">
+        <v>4</v>
+      </c>
+      <c r="D22" s="52"/>
+      <c r="E22" s="1">
+        <f t="shared" si="1"/>
+        <v>5.7999999999999996E-2</v>
+      </c>
+      <c r="F22" s="52"/>
+      <c r="G22" s="1">
+        <f t="shared" si="2"/>
+        <v>5.9199999999999999E-3</v>
+      </c>
+      <c r="H22" s="1">
+        <f t="shared" si="2"/>
+        <v>2.96E-3</v>
+      </c>
+      <c r="I22" s="1">
+        <f t="shared" si="3"/>
+        <v>5.91</v>
+      </c>
+      <c r="J22" s="52"/>
+      <c r="K22" s="52"/>
+      <c r="L22" s="1">
+        <f t="shared" si="4"/>
+        <v>0.1042</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C23" s="1">
+        <v>5</v>
+      </c>
+      <c r="D23" s="52"/>
+      <c r="E23" s="1">
+        <f t="shared" si="1"/>
+        <v>5.8299999999999998E-2</v>
+      </c>
+      <c r="F23" s="52"/>
+      <c r="G23" s="1">
+        <f t="shared" si="2"/>
+        <v>5.5300000000000002E-3</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" si="2"/>
+        <v>2.7650000000000001E-3</v>
+      </c>
+      <c r="I23" s="1">
+        <f t="shared" si="3"/>
+        <v>6.87</v>
+      </c>
+      <c r="J23" s="52"/>
+      <c r="K23" s="52"/>
+      <c r="L23" s="1">
+        <f t="shared" si="4"/>
+        <v>0.1065</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C24" s="1">
+        <v>6</v>
+      </c>
+      <c r="D24" s="52"/>
+      <c r="E24" s="1">
+        <f t="shared" si="1"/>
+        <v>5.7660000000000003E-2</v>
+      </c>
+      <c r="F24" s="52"/>
+      <c r="G24" s="1">
+        <f t="shared" si="2"/>
+        <v>5.9699999999999996E-3</v>
+      </c>
+      <c r="H24" s="1">
+        <f t="shared" si="2"/>
+        <v>2.9849999999999998E-3</v>
+      </c>
+      <c r="I24" s="1">
+        <f t="shared" si="3"/>
+        <v>6.82</v>
+      </c>
+      <c r="J24" s="52"/>
+      <c r="K24" s="52"/>
+      <c r="L24" s="1">
+        <f t="shared" si="4"/>
+        <v>0.1222</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C25" s="1">
+        <v>7</v>
+      </c>
+      <c r="D25" s="52"/>
+      <c r="E25" s="1">
+        <f t="shared" si="1"/>
+        <v>5.8120000000000005E-2</v>
+      </c>
+      <c r="F25" s="52"/>
+      <c r="G25" s="1">
+        <f t="shared" si="2"/>
+        <v>5.8700000000000002E-3</v>
+      </c>
+      <c r="H25" s="1">
+        <f t="shared" si="2"/>
+        <v>2.9350000000000001E-3</v>
+      </c>
+      <c r="I25" s="1">
+        <f t="shared" si="3"/>
+        <v>6.66</v>
+      </c>
+      <c r="J25" s="52"/>
+      <c r="K25" s="52"/>
+      <c r="L25" s="1">
+        <f t="shared" si="4"/>
+        <v>0.11559999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C26" s="1">
+        <v>8</v>
+      </c>
+      <c r="D26" s="52"/>
+      <c r="E26" s="1">
+        <f t="shared" si="1"/>
+        <v>5.8099999999999999E-2</v>
+      </c>
+      <c r="F26" s="52"/>
+      <c r="G26" s="1">
+        <f t="shared" si="2"/>
+        <v>5.8899999999999994E-3</v>
+      </c>
+      <c r="H26" s="1">
+        <f t="shared" si="2"/>
+        <v>2.9449999999999997E-3</v>
+      </c>
+      <c r="I26" s="1">
+        <f t="shared" si="3"/>
+        <v>7.56</v>
+      </c>
+      <c r="J26" s="52"/>
+      <c r="K26" s="52"/>
+      <c r="L26" s="1">
+        <f t="shared" si="4"/>
+        <v>0.13200000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C27" s="1">
+        <v>9</v>
+      </c>
+      <c r="D27" s="52"/>
+      <c r="E27" s="1">
+        <f t="shared" si="1"/>
+        <v>5.7640000000000004E-2</v>
+      </c>
+      <c r="F27" s="52"/>
+      <c r="G27" s="1">
+        <f t="shared" si="2"/>
+        <v>5.9800000000000001E-3</v>
+      </c>
+      <c r="H27" s="1">
+        <f t="shared" si="2"/>
+        <v>2.99E-3</v>
+      </c>
+      <c r="I27" s="1">
+        <f t="shared" si="3"/>
+        <v>6.81</v>
+      </c>
+      <c r="J27" s="52"/>
+      <c r="K27" s="52"/>
+      <c r="L27" s="1">
+        <f t="shared" si="4"/>
+        <v>0.12239999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C28" s="1">
+        <v>10</v>
+      </c>
+      <c r="D28" s="53"/>
+      <c r="E28" s="1">
+        <f t="shared" si="1"/>
+        <v>5.8019999999999995E-2</v>
+      </c>
+      <c r="F28" s="53"/>
+      <c r="G28" s="1">
+        <f t="shared" si="2"/>
+        <v>5.94E-3</v>
+      </c>
+      <c r="H28" s="1">
+        <f t="shared" si="2"/>
+        <v>2.97E-3</v>
+      </c>
+      <c r="I28" s="1">
+        <f t="shared" si="3"/>
+        <v>5.38</v>
+      </c>
+      <c r="J28" s="53"/>
+      <c r="K28" s="53"/>
+      <c r="L28" s="1">
+        <f t="shared" si="4"/>
+        <v>9.5500000000000002E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C29" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H29" s="36">
+        <f>AVERAGE(H19:H28)</f>
+        <v>2.941E-3</v>
+      </c>
+      <c r="L29" s="1">
+        <f>ROUND(AVERAGE(L19:L28),4)</f>
+        <v>0.1123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" ht="18" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I32" s="35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>5.8013999999999996E-2</v>
+      </c>
+      <c r="B33">
+        <v>2.9</v>
+      </c>
+      <c r="C33" s="38">
+        <f t="shared" ref="C33:C42" si="5">POWER(H19,2)</f>
+        <v>8.4099999999999991E-6</v>
+      </c>
+      <c r="D33" s="1">
+        <f>$T$19</f>
+        <v>9.8066499999999994</v>
+      </c>
+      <c r="E33" s="1">
+        <f>$J$19-$K$19</f>
+        <v>367.95744665941288</v>
+      </c>
+      <c r="F33" s="1">
+        <f t="shared" ref="F33:F42" si="6">I19</f>
+        <v>6.34</v>
+      </c>
+      <c r="G33" s="1">
+        <f>$D$19</f>
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="H33" s="1">
+        <f t="shared" ref="H33:H42" si="7">H19/$F$19</f>
+        <v>4.9987933946978313E-2</v>
+      </c>
+      <c r="I33" s="1">
+        <f t="shared" ref="I33:I42" si="8">(2*C33*D33*E33*F33)/(9*G33*(1+(2.4*H33)))</f>
+        <v>0.10753649210678601</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>5.8013999999999996E-2</v>
+      </c>
+      <c r="B34">
+        <v>2.97</v>
+      </c>
+      <c r="C34" s="38">
+        <f t="shared" si="5"/>
+        <v>8.8209000000000005E-6</v>
+      </c>
+      <c r="D34" s="1">
+        <f t="shared" ref="D34:D42" si="9">$T$19</f>
+        <v>9.8066499999999994</v>
+      </c>
+      <c r="E34" s="1">
+        <f t="shared" ref="E34:E42" si="10">$J$19-$K$19</f>
+        <v>367.95744665941288</v>
+      </c>
+      <c r="F34" s="1">
+        <f t="shared" si="6"/>
+        <v>5.15</v>
+      </c>
+      <c r="G34" s="1">
+        <f t="shared" ref="G34:G42" si="11">$D$19</f>
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="H34" s="1">
+        <f t="shared" si="7"/>
+        <v>5.1194539249146763E-2</v>
+      </c>
+      <c r="I34" s="1">
+        <f t="shared" si="8"/>
+        <v>9.1383808848443354E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>5.8013999999999996E-2</v>
+      </c>
+      <c r="B35">
+        <v>2.99</v>
+      </c>
+      <c r="C35" s="38">
+        <f t="shared" si="5"/>
+        <v>8.940100000000001E-6</v>
+      </c>
+      <c r="D35" s="1">
+        <f t="shared" si="9"/>
+        <v>9.8066499999999994</v>
+      </c>
+      <c r="E35" s="1">
+        <f t="shared" si="10"/>
+        <v>367.95744665941288</v>
+      </c>
+      <c r="F35" s="1">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="G35" s="1">
+        <f t="shared" si="11"/>
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="H35" s="1">
+        <f t="shared" si="7"/>
+        <v>5.1539283621194885E-2</v>
+      </c>
+      <c r="I35" s="1">
+        <f t="shared" si="8"/>
+        <v>0.12579681673671783</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>5.8013999999999996E-2</v>
+      </c>
+      <c r="B36">
+        <v>2.96</v>
+      </c>
+      <c r="C36" s="38">
+        <f t="shared" si="5"/>
+        <v>8.7615999999999993E-6</v>
+      </c>
+      <c r="D36" s="1">
+        <f t="shared" si="9"/>
+        <v>9.8066499999999994</v>
+      </c>
+      <c r="E36" s="1">
+        <f t="shared" si="10"/>
+        <v>367.95744665941288</v>
+      </c>
+      <c r="F36" s="1">
+        <f t="shared" si="6"/>
+        <v>5.91</v>
+      </c>
+      <c r="G36" s="1">
+        <f t="shared" si="11"/>
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="H36" s="1">
+        <f t="shared" si="7"/>
+        <v>5.1022167063122695E-2</v>
+      </c>
+      <c r="I36" s="1">
+        <f t="shared" si="8"/>
+        <v>0.10420296233778492</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>5.8013999999999996E-2</v>
+      </c>
+      <c r="B37">
+        <v>2.7650000000000001</v>
+      </c>
+      <c r="C37" s="38">
+        <f t="shared" si="5"/>
+        <v>7.645225000000001E-6</v>
+      </c>
+      <c r="D37" s="1">
+        <f t="shared" si="9"/>
+        <v>9.8066499999999994</v>
+      </c>
+      <c r="E37" s="1">
+        <f t="shared" si="10"/>
+        <v>367.95744665941288</v>
+      </c>
+      <c r="F37" s="1">
+        <f t="shared" si="6"/>
+        <v>6.87</v>
+      </c>
+      <c r="G37" s="1">
+        <f t="shared" si="11"/>
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="H37" s="1">
+        <f t="shared" si="7"/>
+        <v>4.7660909435653466E-2</v>
+      </c>
+      <c r="I37" s="1">
+        <f t="shared" si="8"/>
+        <v>0.10646054742754973</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>5.8013999999999996E-2</v>
+      </c>
+      <c r="B38">
+        <v>2.9849999999999999</v>
+      </c>
+      <c r="C38" s="38">
+        <f t="shared" si="5"/>
+        <v>8.9102249999999982E-6</v>
+      </c>
+      <c r="D38" s="1">
+        <f t="shared" si="9"/>
+        <v>9.8066499999999994</v>
+      </c>
+      <c r="E38" s="1">
+        <f t="shared" si="10"/>
+        <v>367.95744665941288</v>
+      </c>
+      <c r="F38" s="1">
+        <f t="shared" si="6"/>
+        <v>6.82</v>
+      </c>
+      <c r="G38" s="1">
+        <f t="shared" si="11"/>
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="H38" s="1">
+        <f t="shared" si="7"/>
+        <v>5.1453097528182855E-2</v>
+      </c>
+      <c r="I38" s="1">
+        <f t="shared" si="8"/>
+        <v>0.12217496732687939</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>5.8013999999999996E-2</v>
+      </c>
+      <c r="B39">
+        <v>2.9350000000000001</v>
+      </c>
+      <c r="C39" s="38">
+        <f t="shared" si="5"/>
+        <v>8.6142250000000014E-6</v>
+      </c>
+      <c r="D39" s="1">
+        <f t="shared" si="9"/>
+        <v>9.8066499999999994</v>
+      </c>
+      <c r="E39" s="1">
+        <f t="shared" si="10"/>
+        <v>367.95744665941288</v>
+      </c>
+      <c r="F39" s="1">
+        <f t="shared" si="6"/>
+        <v>6.66</v>
+      </c>
+      <c r="G39" s="1">
+        <f t="shared" si="11"/>
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="H39" s="1">
+        <f t="shared" si="7"/>
+        <v>5.0591236598062542E-2</v>
+      </c>
+      <c r="I39" s="1">
+        <f t="shared" si="8"/>
+        <v>0.11555798172279318</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>5.8013999999999996E-2</v>
+      </c>
+      <c r="B40">
+        <v>2.9449999999999998</v>
+      </c>
+      <c r="C40" s="38">
+        <f t="shared" si="5"/>
+        <v>8.6730249999999982E-6</v>
+      </c>
+      <c r="D40" s="1">
+        <f t="shared" si="9"/>
+        <v>9.8066499999999994</v>
+      </c>
+      <c r="E40" s="1">
+        <f t="shared" si="10"/>
+        <v>367.95744665941288</v>
+      </c>
+      <c r="F40" s="1">
+        <f t="shared" si="6"/>
+        <v>7.56</v>
+      </c>
+      <c r="G40" s="1">
+        <f t="shared" si="11"/>
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="H40" s="1">
+        <f t="shared" si="7"/>
+        <v>5.0763608784086596E-2</v>
+      </c>
+      <c r="I40" s="1">
+        <f t="shared" si="8"/>
+        <v>0.13202060514334538</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>5.8013999999999996E-2</v>
+      </c>
+      <c r="B41">
+        <v>2.99</v>
+      </c>
+      <c r="C41" s="38">
+        <f t="shared" si="5"/>
+        <v>8.940100000000001E-6</v>
+      </c>
+      <c r="D41" s="1">
+        <f t="shared" si="9"/>
+        <v>9.8066499999999994</v>
+      </c>
+      <c r="E41" s="1">
+        <f t="shared" si="10"/>
+        <v>367.95744665941288</v>
+      </c>
+      <c r="F41" s="1">
+        <f t="shared" si="6"/>
+        <v>6.81</v>
+      </c>
+      <c r="G41" s="1">
+        <f t="shared" si="11"/>
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="H41" s="1">
+        <f t="shared" si="7"/>
+        <v>5.1539283621194885E-2</v>
+      </c>
+      <c r="I41" s="1">
+        <f t="shared" si="8"/>
+        <v>0.1223823317110069</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>5.8014000000000003E-2</v>
+      </c>
+      <c r="B42">
+        <v>2.97</v>
+      </c>
+      <c r="C42" s="38">
+        <f t="shared" si="5"/>
+        <v>8.8209000000000005E-6</v>
+      </c>
+      <c r="D42" s="1">
+        <f t="shared" si="9"/>
+        <v>9.8066499999999994</v>
+      </c>
+      <c r="E42" s="1">
+        <f t="shared" si="10"/>
+        <v>367.95744665941288</v>
+      </c>
+      <c r="F42" s="1">
+        <f t="shared" si="6"/>
+        <v>5.38</v>
+      </c>
+      <c r="G42" s="1">
+        <f t="shared" si="11"/>
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="H42" s="1">
+        <f t="shared" si="7"/>
+        <v>5.1194539249146763E-2</v>
+      </c>
+      <c r="I42" s="1">
+        <f t="shared" si="8"/>
+        <v>9.5465027496043742E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F43" s="37"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C46" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I46" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C47" s="1">
+        <v>1</v>
+      </c>
+      <c r="D47" s="1">
+        <v>0.1075</v>
+      </c>
+      <c r="E47" s="1">
+        <f>((20*B33*F33*D33*E33)*(45*A33*G33+108*B33*G33)-(10*C33*F33*A33*D33*E33)*108) / POWER((45*G33*A33+108*G33*B33),2)</f>
+        <v>11835.33053373598</v>
+      </c>
+      <c r="F47" s="1">
+        <f>N47</f>
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <f>ROUND((10*C33*D33*A33*E33)/(45*G33*A33+108*G33*B33),8)</f>
+        <v>1.5703000000000001E-4</v>
+      </c>
+      <c r="H47" s="1">
+        <f>(10*C33*F33*D33*A33*E33)*(45*A33+108*B33)/POWER((45*G33*A33+108*B33),2)</f>
+        <v>3.572343178608313E-4</v>
+      </c>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C48" s="1">
+        <v>2</v>
+      </c>
+      <c r="D48" s="1">
+        <v>9.1399999999999995E-2</v>
+      </c>
+      <c r="E48" s="1">
+        <f t="shared" ref="E48:E56" si="12">((20*B34*F34*D34*E34)*(45*A34*G34+108*B34*G34)-(10*C34*F34*A34*D34*E34)*108) / POWER((45*G34*A34+108*G34*B34),2)</f>
+        <v>9615.7460488135166</v>
+      </c>
+      <c r="F48" s="1"/>
+      <c r="G48">
+        <f t="shared" ref="G48:G56" si="13">ROUND((10*C34*D34*A34*E34)/(45*G34*A34+108*G34*B34),8)</f>
+        <v>1.6086E-4</v>
+      </c>
+      <c r="H48" s="1">
+        <f t="shared" ref="H48:H56" si="14">(10*C34*F34*D34*A34*E34)*(45*A34+108*B34)/POWER((45*G34*A34+108*B34),2)</f>
+        <v>2.9717027980166315E-4</v>
+      </c>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+    </row>
+    <row r="49" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C49" s="1">
+        <v>3</v>
+      </c>
+      <c r="D49" s="1">
+        <v>0.1258</v>
+      </c>
+      <c r="E49" s="1">
+        <f t="shared" si="12"/>
+        <v>13070.651916838009</v>
+      </c>
+      <c r="F49" s="1"/>
+      <c r="G49">
+        <f t="shared" si="13"/>
+        <v>1.6195000000000001E-4</v>
+      </c>
+      <c r="H49" s="1">
+        <f t="shared" si="14"/>
+        <v>4.0663448691735454E-4</v>
+      </c>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+    </row>
+    <row r="50" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C50" s="1">
+        <v>4</v>
+      </c>
+      <c r="D50" s="1">
+        <v>0.1042</v>
+      </c>
+      <c r="E50" s="1">
+        <f t="shared" si="12"/>
+        <v>11034.467809732463</v>
+      </c>
+      <c r="F50" s="1"/>
+      <c r="G50">
+        <f t="shared" si="13"/>
+        <v>1.6030999999999999E-4</v>
+      </c>
+      <c r="H50" s="1">
+        <f t="shared" si="14"/>
+        <v>3.3987895765752023E-4</v>
+      </c>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+    </row>
+    <row r="51" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C51" s="1">
+        <v>5</v>
+      </c>
+      <c r="D51" s="1">
+        <v>0.1065</v>
+      </c>
+      <c r="E51" s="1">
+        <f t="shared" si="12"/>
+        <v>12819.54532362522</v>
+      </c>
+      <c r="F51" s="1"/>
+      <c r="G51">
+        <f t="shared" si="13"/>
+        <v>1.4966E-4</v>
+      </c>
+      <c r="H51" s="1">
+        <f t="shared" si="14"/>
+        <v>3.6912029870458777E-4</v>
+      </c>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+    </row>
+    <row r="52" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C52" s="1">
+        <v>6</v>
+      </c>
+      <c r="D52" s="1">
+        <v>0.1222</v>
+      </c>
+      <c r="E52" s="1">
+        <f t="shared" si="12"/>
+        <v>12734.378375675102</v>
+      </c>
+      <c r="F52" s="1"/>
+      <c r="G52">
+        <f t="shared" si="13"/>
+        <v>1.6166999999999999E-4</v>
+      </c>
+      <c r="H52" s="1">
+        <f t="shared" si="14"/>
+        <v>3.9551718737888456E-4</v>
+      </c>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+    </row>
+    <row r="53" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C53" s="1">
+        <v>7</v>
+      </c>
+      <c r="D53" s="1">
+        <v>0.11559999999999999</v>
+      </c>
+      <c r="E53" s="1">
+        <f t="shared" si="12"/>
+        <v>12433.923081538562</v>
+      </c>
+      <c r="F53" s="1"/>
+      <c r="G53">
+        <f t="shared" si="13"/>
+        <v>1.5893999999999999E-4</v>
+      </c>
+      <c r="H53" s="1">
+        <f t="shared" si="14"/>
+        <v>3.7978341718217289E-4</v>
+      </c>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+    </row>
+    <row r="54" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C54" s="1">
+        <v>8</v>
+      </c>
+      <c r="D54" s="1">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="E54" s="1">
+        <f t="shared" si="12"/>
+        <v>14114.574459202493</v>
+      </c>
+      <c r="F54" s="1"/>
+      <c r="G54">
+        <f t="shared" si="13"/>
+        <v>1.5949000000000001E-4</v>
+      </c>
+      <c r="H54" s="1">
+        <f t="shared" si="14"/>
+        <v>4.3257090930654495E-4</v>
+      </c>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+    </row>
+    <row r="55" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C55" s="1">
+        <v>9</v>
+      </c>
+      <c r="D55" s="1">
+        <v>0.12239999999999999</v>
+      </c>
+      <c r="E55" s="1">
+        <f t="shared" si="12"/>
+        <v>12715.877079095262</v>
+      </c>
+      <c r="F55" s="1"/>
+      <c r="G55">
+        <f t="shared" si="13"/>
+        <v>1.6195000000000001E-4</v>
+      </c>
+      <c r="H55" s="1">
+        <f t="shared" si="14"/>
+        <v>3.9559726512959777E-4</v>
+      </c>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+    </row>
+    <row r="56" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C56" s="1">
+        <v>10</v>
+      </c>
+      <c r="D56" s="1">
+        <v>9.5500000000000002E-2</v>
+      </c>
+      <c r="E56" s="1">
+        <f t="shared" si="12"/>
+        <v>10045.187134488682</v>
+      </c>
+      <c r="F56" s="1"/>
+      <c r="G56">
+        <f t="shared" si="13"/>
+        <v>1.6086E-4</v>
+      </c>
+      <c r="H56" s="1">
+        <f t="shared" si="14"/>
+        <v>3.1044196220057248E-4</v>
+      </c>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="K19:K28"/>
+    <mergeCell ref="D19:D28"/>
+    <mergeCell ref="F19:F28"/>
+    <mergeCell ref="F5:F14"/>
+    <mergeCell ref="D5:D14"/>
+    <mergeCell ref="J19:J28"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>